<commit_message>
Updates for adding EDT, etc
</commit_message>
<xml_diff>
--- a/Data/Okanogan_AU_Reach_Crosswalk.xlsx
+++ b/Data/Okanogan_AU_Reach_Crosswalk.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E091A-299E-428C-AEEF-10DC02D49EF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E5D83D-5465-4DE2-8309-B745E11C099D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="648" yWindow="756" windowWidth="19992" windowHeight="11508" xr2:uid="{C5E7F2ED-6596-48A9-B90D-5FCE0460D933}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5E7F2ED-6596-48A9-B90D-5FCE0460D933}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$132</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="303">
   <si>
     <t>Aeneas Creek 01</t>
   </si>
@@ -913,6 +916,36 @@
   </si>
   <si>
     <t>Loup Loup 16-4.1 (falls)</t>
+  </si>
+  <si>
+    <t>Aeneas Creek-DS</t>
+  </si>
+  <si>
+    <t>Antoine Creek-Lower DS</t>
+  </si>
+  <si>
+    <t>Bonaparte Creek-Lower DS</t>
+  </si>
+  <si>
+    <t>Loup Loup Creek-Lower DS</t>
+  </si>
+  <si>
+    <t>Omak Creek-Lower US</t>
+  </si>
+  <si>
+    <t>Siwash Creek-Lower DS</t>
+  </si>
+  <si>
+    <t>Tunk Creek-Lower DS</t>
+  </si>
+  <si>
+    <t>Omak Creek-Middle DS</t>
+  </si>
+  <si>
+    <t>Okanogan-Alkali Lake</t>
+  </si>
+  <si>
+    <t>Okanogan-Davis Canyon</t>
   </si>
 </sst>
 </file>
@@ -956,7 +989,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -964,13 +997,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1287,14 +1333,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F339BF-C3F0-4145-B7A6-05FCE79631DF}">
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
     <col min="3" max="3" width="27.21875" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
   </cols>
@@ -1326,6 +1372,9 @@
       <c r="C2" t="s">
         <v>238</v>
       </c>
+      <c r="D2" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1337,1351 +1386,1498 @@
       <c r="C3" t="s">
         <v>239</v>
       </c>
+      <c r="D3" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>247</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>241</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>242</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>243</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>244</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>235</v>
+        <v>245</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>246</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>167</v>
+        <v>248</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>230</v>
+      </c>
+      <c r="D12" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>231</v>
+      </c>
+      <c r="D13" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>242</v>
+        <v>232</v>
+      </c>
+      <c r="D14" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
+        <v>233</v>
+      </c>
+      <c r="D15" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+      <c r="D16" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+      <c r="D17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+      <c r="D18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>272</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>273</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" t="s">
+        <v>276</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>277</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>278</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
+        <v>287</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" t="s">
+        <v>287</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="s">
+        <v>288</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>284</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E41" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
+        <v>284</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E42" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>35</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B43" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C43" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="D43" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B44" t="s">
         <v>36</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C44" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="D44" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C45" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D45" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>40</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B46" t="s">
         <v>39</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C46" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="D46" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>41</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B47" t="s">
         <v>39</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C47" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="D47" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B48" t="s">
         <v>39</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C48" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="D48" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>43</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B49" t="s">
         <v>39</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C49" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="D49" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B50" t="s">
         <v>39</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C50" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="D50" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B51" t="s">
         <v>39</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C51" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="D51" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>47</v>
-      </c>
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>61</v>
       </c>
       <c r="B52" t="s">
         <v>48</v>
       </c>
       <c r="C52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>62</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B73" t="s">
         <v>30</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C73" t="s">
         <v>207</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E73" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>63</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B74" t="s">
         <v>30</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C74" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>64</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B75" t="s">
         <v>30</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C75" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>65</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B77" t="s">
         <v>66</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C77" t="s">
         <v>176</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E77" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B78" t="s">
         <v>66</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C78" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>68</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B79" t="s">
         <v>66</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C79" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>69</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B80" t="s">
         <v>66</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C80" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>71</v>
-      </c>
-      <c r="B61" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>72</v>
-      </c>
-      <c r="B62" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>75</v>
-      </c>
-      <c r="B65" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>77</v>
-      </c>
-      <c r="B67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>78</v>
-      </c>
-      <c r="B68" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>79</v>
-      </c>
-      <c r="B69" t="s">
-        <v>13</v>
-      </c>
-      <c r="C69" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B72" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>85</v>
-      </c>
-      <c r="B74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>86</v>
-      </c>
-      <c r="B75" t="s">
-        <v>83</v>
-      </c>
-      <c r="C75" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" t="s">
-        <v>83</v>
-      </c>
-      <c r="C76" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>88</v>
-      </c>
-      <c r="B77" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>89</v>
-      </c>
-      <c r="B78" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>92</v>
-      </c>
-      <c r="B80" t="s">
-        <v>91</v>
-      </c>
-      <c r="C80" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B81" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C81" t="s">
-        <v>268</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
-        <v>269</v>
+        <v>182</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="B83" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C83" t="s">
-        <v>270</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C84" t="s">
-        <v>271</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="C85" t="s">
-        <v>272</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="C86" t="s">
-        <v>273</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>274</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="C88" t="s">
-        <v>275</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>276</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>277</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>278</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>279</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>280</v>
+        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B94" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C94" t="s">
-        <v>281</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C95" t="s">
-        <v>282</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" t="s">
+        <v>83</v>
+      </c>
+      <c r="C96" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>87</v>
+      </c>
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
+      <c r="C98" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" t="s">
+        <v>83</v>
+      </c>
+      <c r="C99" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>89</v>
+      </c>
+      <c r="B100" t="s">
+        <v>83</v>
+      </c>
+      <c r="C100" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>110</v>
-      </c>
-      <c r="B96" t="s">
-        <v>111</v>
-      </c>
-      <c r="C96" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>112</v>
-      </c>
-      <c r="B97" t="s">
-        <v>111</v>
-      </c>
-      <c r="C97" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>113</v>
-      </c>
-      <c r="B98" t="s">
-        <v>111</v>
-      </c>
-      <c r="C98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>114</v>
-      </c>
-      <c r="B99" t="s">
-        <v>111</v>
-      </c>
-      <c r="C99" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>115</v>
-      </c>
-      <c r="B100" t="s">
-        <v>111</v>
-      </c>
-      <c r="C100" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>116</v>
       </c>
       <c r="B101" t="s">
         <v>111</v>
       </c>
       <c r="C101" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B102" t="s">
         <v>111</v>
       </c>
       <c r="C102" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B103" t="s">
         <v>111</v>
       </c>
       <c r="C103" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B104" t="s">
         <v>111</v>
       </c>
       <c r="C104" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B105" t="s">
         <v>111</v>
       </c>
       <c r="C105" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B106" t="s">
         <v>111</v>
       </c>
       <c r="C106" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B107" t="s">
         <v>111</v>
       </c>
       <c r="C107" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B108" t="s">
         <v>111</v>
       </c>
       <c r="C108" t="s">
-        <v>261</v>
-      </c>
-      <c r="E108" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B109" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="C109" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B110" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B111" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C112" t="s">
-        <v>222</v>
+        <v>260</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B113" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>223</v>
+        <v>261</v>
+      </c>
+      <c r="E113" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B114" t="s">
         <v>126</v>
       </c>
       <c r="C114" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B115" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C115" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B116" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C116" t="s">
-        <v>287</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B117" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C117" t="s">
-        <v>287</v>
+        <v>223</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B118" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C118" t="s">
-        <v>288</v>
+        <v>224</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C119" t="s">
-        <v>284</v>
-      </c>
-      <c r="E119" t="s">
-        <v>285</v>
+        <v>217</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C120" t="s">
-        <v>284</v>
-      </c>
-      <c r="E120" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="B121" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C121" t="s">
-        <v>216</v>
+        <v>280</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="B122" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="C122" t="s">
-        <v>217</v>
+        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="B123" t="s">
         <v>106</v>
       </c>
       <c r="C123" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B124" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="C124" t="s">
-        <v>240</v>
+        <v>283</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2773,6 +2969,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E132" xr:uid="{1FF114CF-7205-4FA0-9C60-87D210D84E10}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E132">
+      <sortCondition ref="B1:B132"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>